<commit_message>
Addition of the case studies Mob 1 % 2
</commit_message>
<xml_diff>
--- a/lyrio.xlsx
+++ b/lyrio.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/achuat/Documents/Projects/Governance_EnergyScope/EnergyScopePy_dev/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D683404-8F8C-BD4C-9328-B8C9436C2965}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{163944B0-1E3D-5244-9181-97E92480928E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1060" yWindow="-23500" windowWidth="34620" windowHeight="21760" xr2:uid="{BAA1AB20-F9F5-294C-88D8-C5249A4E7D58}"/>
+    <workbookView xWindow="33560" yWindow="-20500" windowWidth="33600" windowHeight="20500" xr2:uid="{BAA1AB20-F9F5-294C-88D8-C5249A4E7D58}"/>
   </bookViews>
   <sheets>
     <sheet name="lyrio" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="174">
   <si>
     <t xml:space="preserve">let end_uses_demand_year['ELECTRICITY_LV','HOUSEHOLDS'] := 11792 ; # </t>
   </si>
@@ -559,6 +559,9 @@
   <si>
     <t>param storage_eff_out :</t>
   </si>
+  <si>
+    <t>s</t>
+  </si>
 </sst>
 </file>
 
@@ -937,10 +940,10 @@
   <dimension ref="A1:AM125"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="81" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B42" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="U2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Z1" sqref="Z1:AL1048576"/>
+      <selection pane="bottomRight" activeCell="Z16" sqref="Z16:Z17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15736,7 +15739,7 @@
   <dimension ref="A1:AG72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="W47" sqref="W47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -18557,8 +18560,8 @@
       <c r="V47">
         <v>0</v>
       </c>
-      <c r="W47">
-        <v>0</v>
+      <c r="W47" t="s">
+        <v>173</v>
       </c>
       <c r="X47">
         <v>0</v>

</xml_diff>